<commit_message>
API Automation Framework Part-V Added Logging for CowinAPI TC's
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>HWC NEWAL BANGARMAU</t>
+  </si>
+  <si>
+    <t>Apollo</t>
   </si>
   <si>
     <t>Kanpur Nagar</t>
@@ -1514,10 +1517,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="10">
-        <v>226003</v>
+        <v>226012</v>
       </c>
       <c r="D6" t="s" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -1545,7 +1548,7 @@
         <v>663</v>
       </c>
       <c r="D8" t="s" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
@@ -1559,7 +1562,7 @@
         <v>670</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
@@ -1571,7 +1574,7 @@
       </c>
       <c r="C10" s="9"/>
       <c r="D10" t="s" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">

</xml_diff>